<commit_message>
update my log and add ip address
</commit_message>
<xml_diff>
--- a/Doc_log/log_201508030113_张玉龙.xlsx
+++ b/Doc_log/log_201508030113_张玉龙.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="9924"/>
+    <workbookView windowWidth="15455" windowHeight="8387"/>
   </bookViews>
   <sheets>
     <sheet name="日志" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
   <si>
     <t>日期</t>
   </si>
@@ -42,6 +42,18 @@
   </si>
   <si>
     <t>需要学习火车收集器的使用规则，开始收集高校图书馆信息</t>
+  </si>
+  <si>
+    <t>14：00-16：50 20：00-21：00</t>
+  </si>
+  <si>
+    <t>明确组员分工以及需要解决的技术难题，明白自己的任务</t>
+  </si>
+  <si>
+    <t>初步分工完成</t>
+  </si>
+  <si>
+    <t>收集高校图书馆的url</t>
   </si>
   <si>
     <t>周次</t>
@@ -55,12 +67,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,22 +82,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -98,38 +125,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,34 +141,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -181,7 +156,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -196,25 +171,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,187 +234,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -420,50 +425,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -491,6 +452,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -502,6 +487,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,154 +530,157 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
@@ -1028,17 +1036,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="10.7777777777778"/>
-    <col min="2" max="2" width="16.4444444444444" customWidth="1"/>
-    <col min="3" max="3" width="15.8888888888889" customWidth="1"/>
+    <col min="2" max="2" width="16.4444444444444" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.8888888888889" customWidth="1"/>
     <col min="4" max="4" width="21.8888888888889" customWidth="1"/>
     <col min="5" max="5" width="18.3333333333333" customWidth="1"/>
   </cols>
@@ -1047,7 +1055,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -1061,20 +1069,37 @@
       </c>
     </row>
     <row r="2" ht="75" customHeight="1" spans="1:5">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>43278</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" ht="28.8" spans="1:5">
+      <c r="A3" s="2">
+        <v>43279</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1100,7 +1125,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1109,7 +1134,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update my log and add zzti-data
</commit_message>
<xml_diff>
--- a/Doc_log/log_201508030113_张玉龙.xlsx
+++ b/Doc_log/log_201508030113_张玉龙.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15455" windowHeight="8387"/>
+    <workbookView windowWidth="22943" windowHeight="9924"/>
   </bookViews>
   <sheets>
     <sheet name="日志" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23">
   <si>
     <t>日期</t>
   </si>
@@ -54,6 +54,30 @@
   </si>
   <si>
     <t>收集高校图书馆的url</t>
+  </si>
+  <si>
+    <t>8：00-11：00</t>
+  </si>
+  <si>
+    <t>爬取中原工学院的图书馆新闻页</t>
+  </si>
+  <si>
+    <t>爬虫基本完成，输出格式有待改进</t>
+  </si>
+  <si>
+    <t>继续学习爬虫，爬取其他学校</t>
+  </si>
+  <si>
+    <t>14:30-16：00</t>
+  </si>
+  <si>
+    <t>学习requests这个库的知识</t>
+  </si>
+  <si>
+    <t>学习了一部分，还需要继续学习</t>
+  </si>
+  <si>
+    <t>明天的任务根据教程搭建自己的节点</t>
   </si>
   <si>
     <t>周次</t>
@@ -67,10 +91,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -88,9 +112,122 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -104,122 +241,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -234,187 +258,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,6 +449,17 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -439,39 +474,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -495,18 +497,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,6 +525,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -533,10 +557,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -548,134 +572,134 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -686,6 +710,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1036,13 +1063,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="10.7777777777778"/>
     <col min="2" max="2" width="16.4444444444444" style="1" customWidth="1"/>
@@ -1075,13 +1102,13 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1100,6 +1127,40 @@
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" ht="28.8" spans="1:5">
+      <c r="A4" s="2">
+        <v>43280</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" ht="28.8" spans="1:5">
+      <c r="A5" s="2">
+        <v>43280</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1125,7 +1186,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1134,7 +1195,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update my log about ssh problems
</commit_message>
<xml_diff>
--- a/Doc_log/log_201508030113_张玉龙.xlsx
+++ b/Doc_log/log_201508030113_张玉龙.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
   <si>
     <t>日期</t>
   </si>
@@ -99,6 +99,18 @@
   </si>
   <si>
     <t>没有进行获取master公钥的操作，还需要进一步改善，实现与控制节点的链接，建立spark集群。</t>
+  </si>
+  <si>
+    <t>14：00-16：40</t>
+  </si>
+  <si>
+    <t>与中心节点进行连接，将他的公钥加到自己的虚拟机上，使其可以通过ssh控制自己的节点以及spark环境的启动</t>
+  </si>
+  <si>
+    <t>出现无法ssh连接的情款，通过分析查找，发现在校网的局域网中两台主机是无法互相访问的，将配置文件的IP地址换为实验室的局域网，解决此问题，可以访问控制</t>
+  </si>
+  <si>
+    <t>除了遇到的访问问题还有虚拟机与window系统端口映射问题，通过查找解决了ssh问题，将中心控制节点的公钥添加到自己的虚拟机中，准备通过中央控制启动spark集群</t>
   </si>
   <si>
     <t>周次</t>
@@ -113,9 +125,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -128,6 +140,21 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,15 +175,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,8 +206,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -193,14 +238,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -217,23 +254,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,22 +269,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -279,187 +291,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,6 +482,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -483,25 +510,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,32 +559,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -578,10 +590,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -590,137 +602,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -731,6 +743,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1084,13 +1099,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="13.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="18.6666666666667" style="1" customWidth="1"/>
@@ -1150,7 +1165,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" ht="28.8" spans="1:5">
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>43280</v>
       </c>
@@ -1167,7 +1182,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" ht="28.8" spans="1:5">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>43280</v>
       </c>
@@ -1184,7 +1199,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" ht="57.6" spans="1:4">
+    <row r="6" ht="43.2" spans="1:4">
       <c r="A6" s="2">
         <v>43281</v>
       </c>
@@ -1198,21 +1213,38 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" ht="86.4" spans="1:5">
+    <row r="7" ht="57.6" spans="1:5">
       <c r="A7" s="2">
         <v>43281</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="8" ht="72" spans="1:5">
+      <c r="A8" s="2">
+        <v>43283</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1238,7 +1270,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1247,7 +1279,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update my log and delete some file
</commit_message>
<xml_diff>
--- a/Doc_log/log_201508030113_张玉龙.xlsx
+++ b/Doc_log/log_201508030113_张玉龙.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38">
   <si>
     <t>日期</t>
   </si>
@@ -111,6 +111,18 @@
   </si>
   <si>
     <t>除了遇到的访问问题还有虚拟机与window系统端口映射问题，通过查找解决了ssh问题，将中心控制节点的公钥添加到自己的虚拟机中，准备通过中央控制启动spark集群</t>
+  </si>
+  <si>
+    <t>12：00-15：00</t>
+  </si>
+  <si>
+    <t>听取老师的建议后，用爬虫爬取图书馆的新闻，写了一个爬取高校图书馆的通用代码，完成数据搜集</t>
+  </si>
+  <si>
+    <t>写了一个代码模型，顺利的爬取了中原工学院图书馆的新闻信息，删除了以前用信息搜索软件搜集的信息以及相关文档，主要是那些软件不够便捷与收费</t>
+  </si>
+  <si>
+    <t>写好了代码后进行量产，需要先搜集高校此网页的IP地址以及分析其url规则</t>
   </si>
   <si>
     <t>周次</t>
@@ -124,10 +136,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -138,6 +150,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -146,15 +220,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -175,9 +256,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -185,22 +265,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,7 +273,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -222,61 +287,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -291,187 +303,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -485,76 +497,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -577,8 +524,73 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -590,10 +602,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -602,133 +614,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1099,13 +1111,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="13.6666666666667" customWidth="1"/>
     <col min="2" max="2" width="18.6666666666667" style="1" customWidth="1"/>
@@ -1240,11 +1252,28 @@
       <c r="C8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="9" ht="72" spans="1:5">
+      <c r="A9" s="2">
+        <v>43284</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1270,7 +1299,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -1279,7 +1308,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>